<commit_message>
Define Table và Data SQL đã update
</commit_message>
<xml_diff>
--- a/Database/DataSQL-Demo.xlsx
+++ b/Database/DataSQL-Demo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,12 @@
     <sheet name="user_group" sheetId="2" r:id="rId3"/>
     <sheet name="function" sheetId="5" r:id="rId4"/>
     <sheet name="permission" sheetId="4" r:id="rId5"/>
+    <sheet name="room_type" sheetId="6" r:id="rId6"/>
+    <sheet name="room" sheetId="7" r:id="rId7"/>
+    <sheet name="status" sheetId="8" r:id="rId8"/>
+    <sheet name="reservation" sheetId="9" r:id="rId9"/>
+    <sheet name="reservation_detail" sheetId="10" r:id="rId10"/>
+    <sheet name="guest" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="159">
   <si>
     <t>login_pwd</t>
     <phoneticPr fontId="0"/>
@@ -260,13 +266,268 @@
   </si>
   <si>
     <t>K0002/K0002_4</t>
+  </si>
+  <si>
+    <t>type_name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>varchar(5)</t>
+  </si>
+  <si>
+    <t>room_id</t>
+  </si>
+  <si>
+    <t>floor</t>
+  </si>
+  <si>
+    <t>room_number</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>status_name</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>check_in</t>
+  </si>
+  <si>
+    <t>check_out</t>
+  </si>
+  <si>
+    <t>number_of_room</t>
+  </si>
+  <si>
+    <t>number_of_adult</t>
+  </si>
+  <si>
+    <t>number_of_children</t>
+  </si>
+  <si>
+    <t>create_ymd</t>
+  </si>
+  <si>
+    <t>varchar(8)</t>
+  </si>
+  <si>
+    <t>guest_id</t>
+  </si>
+  <si>
+    <t>interger</t>
+  </si>
+  <si>
+    <t>status_id</t>
+  </si>
+  <si>
+    <t>room_type_id</t>
+  </si>
+  <si>
+    <t>numeric(11,2)</t>
+  </si>
+  <si>
+    <t>varchar(30)</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>varchar(10)</t>
+  </si>
+  <si>
+    <t>status_type</t>
+  </si>
+  <si>
+    <t>varchar(2)</t>
+  </si>
+  <si>
+    <t>varchar(225)</t>
+  </si>
+  <si>
+    <t>reservation_id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>identity_card</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>company_phone</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>varchar(12)</t>
+  </si>
+  <si>
+    <t>Vu Tran Hoang</t>
+  </si>
+  <si>
+    <t>Nguyen Viet Hung</t>
+  </si>
+  <si>
+    <t>Dang Cong Son</t>
+  </si>
+  <si>
+    <t>Tran Ba Quyen</t>
+  </si>
+  <si>
+    <t>Dang Duc Manh</t>
+  </si>
+  <si>
+    <t>Do Hong Khoi</t>
+  </si>
+  <si>
+    <t>Tran Dang Loi</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>RS01</t>
+  </si>
+  <si>
+    <t>RS02</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>RO01</t>
+  </si>
+  <si>
+    <t>RS03</t>
+  </si>
+  <si>
+    <t>RO02</t>
+  </si>
+  <si>
+    <t>RO03</t>
+  </si>
+  <si>
+    <t>RO04</t>
+  </si>
+  <si>
+    <t>Luxury</t>
+  </si>
+  <si>
+    <t>Single room</t>
+  </si>
+  <si>
+    <t>Club</t>
+  </si>
+  <si>
+    <t>Grand Deluxe</t>
+  </si>
+  <si>
+    <t>Royal</t>
+  </si>
+  <si>
+    <t>Club Suite</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>RT01</t>
+  </si>
+  <si>
+    <t>RT02</t>
+  </si>
+  <si>
+    <t>RT03</t>
+  </si>
+  <si>
+    <t>RT04</t>
+  </si>
+  <si>
+    <t>RT05</t>
+  </si>
+  <si>
+    <t>RT06</t>
+  </si>
+  <si>
+    <t>RT07</t>
+  </si>
+  <si>
+    <t>RO001</t>
+  </si>
+  <si>
+    <t>RO002</t>
+  </si>
+  <si>
+    <t>RO003</t>
+  </si>
+  <si>
+    <t>RO004</t>
+  </si>
+  <si>
+    <t>RO005</t>
+  </si>
+  <si>
+    <t>RO006</t>
+  </si>
+  <si>
+    <t>RO007</t>
+  </si>
+  <si>
+    <t>In use</t>
+  </si>
+  <si>
+    <t>On processing</t>
+  </si>
+  <si>
+    <t>Waiting</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Not in use</t>
+  </si>
+  <si>
+    <t>Cleaning</t>
+  </si>
+  <si>
+    <t>Fixing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -386,8 +647,62 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +718,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,10 +752,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -488,9 +810,41 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1161,6 +1515,496 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="23" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4">
+      <c r="B3" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" s="23" t="str">
+        <f xml:space="preserve"> "INSERT INTO tbl_reservation_detail("</f>
+        <v>INSERT INTO tbl_reservation_detail(</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19" s="23" t="str">
+        <f>" "&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;") VALUES('"</f>
+        <v xml:space="preserve"> reservation_id,room_id,create_ymd) VALUES('</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="23" t="str">
+        <f>$C$18&amp;$C$19&amp;C20</f>
+        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,create_ymd) VALUES('1','RO001','');</v>
+      </c>
+      <c r="C20" s="23" t="str">
+        <f>""&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"');"</f>
+        <v>1','RO001','');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="23" t="str">
+        <f t="shared" ref="A21:A26" si="0">$C$18&amp;$C$19&amp;C21</f>
+        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,create_ymd) VALUES('2','RO002','');</v>
+      </c>
+      <c r="C21" s="23" t="str">
+        <f t="shared" ref="C21:C26" si="1">""&amp;B6&amp;"','"&amp;C6&amp;"','"&amp;D6&amp;"');"</f>
+        <v>2','RO002','');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,create_ymd) VALUES('3','RO003','');</v>
+      </c>
+      <c r="C22" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>3','RO003','');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,create_ymd) VALUES('4','RO004','');</v>
+      </c>
+      <c r="C23" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>4','RO004','');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,create_ymd) VALUES('5','RO005','');</v>
+      </c>
+      <c r="C24" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>5','RO005','');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,create_ymd) VALUES('6','RO006','');</v>
+      </c>
+      <c r="C25" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>6','RO006','');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,create_ymd) VALUES('7','RO007','');</v>
+      </c>
+      <c r="C26" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>7','RO007','');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="20" style="23" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="23" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="23" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="23" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="23" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10">
+      <c r="B3" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="1">
+        <v>126491311</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="1">
+        <v>841318413</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="1">
+        <v>511974121</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="1">
+        <v>648413161</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="1">
+        <v>884131988</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="1">
+        <v>651987841</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="1">
+        <v>484216848</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" s="23" t="str">
+        <f xml:space="preserve"> "INSERT INTO tbl_reservation("</f>
+        <v>INSERT INTO tbl_reservation(</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19" s="23" t="str">
+        <f>" "&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;") VALUES('"</f>
+        <v xml:space="preserve"> id,name,phone,mail,identity_card,company,address,company_phone,country) VALUES('</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="23" t="str">
+        <f>$C$18&amp;$C$19&amp;C20</f>
+        <v>INSERT INTO tbl_reservation( id,name,phone,mail,identity_card,company,address,company_phone,country) VALUES('1','Vu Tran Hoang','','','','','','Vietnam');</v>
+      </c>
+      <c r="C20" s="23" t="str">
+        <f>""&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"','"&amp;I5&amp;"','"&amp;J5&amp;"');"</f>
+        <v>1','Vu Tran Hoang','','','','','','Vietnam');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="23" t="str">
+        <f t="shared" ref="A21:A26" si="0">$C$18&amp;$C$19&amp;C21</f>
+        <v>INSERT INTO tbl_reservation( id,name,phone,mail,identity_card,company,address,company_phone,country) VALUES('2','Nguyen Viet Hung','','','','','','Vietnam');</v>
+      </c>
+      <c r="C21" s="23" t="str">
+        <f>""&amp;B6&amp;"','"&amp;C6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"','"&amp;H6&amp;"','"&amp;I6&amp;"','"&amp;J6&amp;"');"</f>
+        <v>2','Nguyen Viet Hung','','','','','','Vietnam');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation( id,name,phone,mail,identity_card,company,address,company_phone,country) VALUES('3','Dang Cong Son','','','','','','Vietnam');</v>
+      </c>
+      <c r="C22" s="23" t="str">
+        <f>""&amp;B7&amp;"','"&amp;C7&amp;"','"&amp;E7&amp;"','"&amp;F7&amp;"','"&amp;G7&amp;"','"&amp;H7&amp;"','"&amp;I7&amp;"','"&amp;J7&amp;"');"</f>
+        <v>3','Dang Cong Son','','','','','','Vietnam');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation( id,name,phone,mail,identity_card,company,address,company_phone,country) VALUES('4','Tran Ba Quyen','','','','','','Vietnam');</v>
+      </c>
+      <c r="C23" s="23" t="str">
+        <f>""&amp;B8&amp;"','"&amp;C8&amp;"','"&amp;E8&amp;"','"&amp;F8&amp;"','"&amp;G8&amp;"','"&amp;H8&amp;"','"&amp;I8&amp;"','"&amp;J8&amp;"');"</f>
+        <v>4','Tran Ba Quyen','','','','','','Vietnam');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation( id,name,phone,mail,identity_card,company,address,company_phone,country) VALUES('5','Dang Duc Manh','','','','','','Vietnam');</v>
+      </c>
+      <c r="C24" s="23" t="str">
+        <f>""&amp;B9&amp;"','"&amp;C9&amp;"','"&amp;E9&amp;"','"&amp;F9&amp;"','"&amp;G9&amp;"','"&amp;H9&amp;"','"&amp;I9&amp;"','"&amp;J9&amp;"');"</f>
+        <v>5','Dang Duc Manh','','','','','','Vietnam');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation( id,name,phone,mail,identity_card,company,address,company_phone,country) VALUES('6','Do Hong Khoi','','','','','','Vietnam');</v>
+      </c>
+      <c r="C25" s="23" t="str">
+        <f>""&amp;B10&amp;"','"&amp;C10&amp;"','"&amp;E10&amp;"','"&amp;F10&amp;"','"&amp;G10&amp;"','"&amp;H10&amp;"','"&amp;I10&amp;"','"&amp;J10&amp;"');"</f>
+        <v>6','Do Hong Khoi','','','','','','Vietnam');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation( id,name,phone,mail,identity_card,company,address,company_phone,country) VALUES('7','Tran Dang Loi','','','','','','Vietnam');</v>
+      </c>
+      <c r="C26" s="23" t="str">
+        <f>""&amp;B11&amp;"','"&amp;C11&amp;"','"&amp;E11&amp;"','"&amp;F11&amp;"','"&amp;G11&amp;"','"&amp;H11&amp;"','"&amp;I11&amp;"','"&amp;J11&amp;"');"</f>
+        <v>7','Tran Dang Loi','','','','','','Vietnam');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I20"/>
@@ -2066,8 +2910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2441,4 +3285,979 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="21" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5">
+      <c r="B3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" s="21" t="str">
+        <f xml:space="preserve"> "INSERT INTO tbl_room_type("</f>
+        <v>INSERT INTO tbl_room_type(</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19" s="21" t="str">
+        <f>" "&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;") VALUES('"</f>
+        <v xml:space="preserve"> room_type_id,type_name,description,price) VALUES('</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="21" t="str">
+        <f>$C$18&amp;$C$19&amp;C20</f>
+        <v>INSERT INTO tbl_room_type( room_type_id,type_name,description,price) VALUES('RT01','Single room','','');</v>
+      </c>
+      <c r="C20" s="21" t="str">
+        <f>""&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"');"</f>
+        <v>RT01','Single room','','');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="21" t="str">
+        <f t="shared" ref="A21:A26" si="0">$C$18&amp;$C$19&amp;C21</f>
+        <v>INSERT INTO tbl_room_type( room_type_id,type_name,description,price) VALUES('RT02','Luxury','','');</v>
+      </c>
+      <c r="C21" s="23" t="str">
+        <f t="shared" ref="C21:C26" si="1">""&amp;B6&amp;"','"&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"');"</f>
+        <v>RT02','Luxury','','');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_room_type( room_type_id,type_name,description,price) VALUES('RT03','Club','','');</v>
+      </c>
+      <c r="C22" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>RT03','Club','','');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_room_type( room_type_id,type_name,description,price) VALUES('RT04','Grand Deluxe','','');</v>
+      </c>
+      <c r="C23" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>RT04','Grand Deluxe','','');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_room_type( room_type_id,type_name,description,price) VALUES('RT05','Royal','','');</v>
+      </c>
+      <c r="C24" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>RT05','Royal','','');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_room_type( room_type_id,type_name,description,price) VALUES('RT06','Club Suite','','');</v>
+      </c>
+      <c r="C25" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>RT06','Club Suite','','');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_room_type( room_type_id,type_name,description,price) VALUES('RT07','Family','','');</v>
+      </c>
+      <c r="C26" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>RT07','Family','','');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="23" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" style="23" customWidth="1"/>
+    <col min="5" max="5" width="9" style="23"/>
+    <col min="6" max="6" width="13" style="23" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="23" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7">
+      <c r="B3" s="30"/>
+      <c r="C3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="31"/>
+      <c r="C4" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="32"/>
+      <c r="C5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="32"/>
+      <c r="C6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="32"/>
+      <c r="C7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" s="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="32"/>
+      <c r="C8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G8" s="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="32"/>
+      <c r="C9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="32"/>
+      <c r="C10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="1">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="32"/>
+      <c r="C11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" s="23" t="str">
+        <f xml:space="preserve"> "INSERT INTO tbl_room("</f>
+        <v>INSERT INTO tbl_room(</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19" s="23" t="str">
+        <f>" "&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;") VALUES('"</f>
+        <v xml:space="preserve"> room_id,room_type_id,floor,status_id,room_number) VALUES('</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="23" t="str">
+        <f>$C$18&amp;$C$19&amp;C20</f>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('','RO001','RT01','1','RO01','101');</v>
+      </c>
+      <c r="C20" s="23" t="str">
+        <f>""&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"');"</f>
+        <v>','RO001','RT01','1','RO01','101');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="23" t="str">
+        <f>$C$18&amp;$C$19&amp;C21</f>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('','RO002','RT01','1','RO01','102');</v>
+      </c>
+      <c r="C21" s="23" t="str">
+        <f>""&amp;B6&amp;"','"&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"');"</f>
+        <v>','RO002','RT01','1','RO01','102');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="23" t="str">
+        <f>$C$18&amp;$C$19&amp;C22</f>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('','RO003','RT03','1','RO02','103');</v>
+      </c>
+      <c r="C22" s="23" t="str">
+        <f>""&amp;B7&amp;"','"&amp;C7&amp;"','"&amp;D7&amp;"','"&amp;E7&amp;"','"&amp;F7&amp;"','"&amp;G7&amp;"');"</f>
+        <v>','RO003','RT03','1','RO02','103');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="23" t="str">
+        <f>$C$18&amp;$C$19&amp;C23</f>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('','RO004','RT04','2','RO02','201');</v>
+      </c>
+      <c r="C23" s="23" t="str">
+        <f>""&amp;B8&amp;"','"&amp;C8&amp;"','"&amp;D8&amp;"','"&amp;E8&amp;"','"&amp;F8&amp;"','"&amp;G8&amp;"');"</f>
+        <v>','RO004','RT04','2','RO02','201');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="23" t="str">
+        <f>$C$18&amp;$C$19&amp;C24</f>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('','RO005','RT05','2','RO02','202');</v>
+      </c>
+      <c r="C24" s="23" t="str">
+        <f>""&amp;B9&amp;"','"&amp;C9&amp;"','"&amp;D9&amp;"','"&amp;E9&amp;"','"&amp;F9&amp;"','"&amp;G9&amp;"');"</f>
+        <v>','RO005','RT05','2','RO02','202');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="23" t="str">
+        <f>$C$18&amp;$C$19&amp;C25</f>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('','RO006','RT05','3','RO03','301');</v>
+      </c>
+      <c r="C25" s="23" t="str">
+        <f>""&amp;B10&amp;"','"&amp;C10&amp;"','"&amp;D10&amp;"','"&amp;E10&amp;"','"&amp;F10&amp;"','"&amp;G10&amp;"');"</f>
+        <v>','RO006','RT05','3','RO03','301');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="23" t="str">
+        <f>$C$18&amp;$C$19&amp;C26</f>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('','RO007','RT07','4','RO03','302');</v>
+      </c>
+      <c r="C26" s="23" t="str">
+        <f>""&amp;B11&amp;"','"&amp;C11&amp;"','"&amp;D11&amp;"','"&amp;E11&amp;"','"&amp;F11&amp;"','"&amp;G11&amp;"');"</f>
+        <v>','RO007','RT07','4','RO03','302');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5">
+      <c r="B3" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" s="23" t="str">
+        <f xml:space="preserve"> "INSERT INTO tbl_status("</f>
+        <v>INSERT INTO tbl_status(</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19" s="23" t="str">
+        <f>" "&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;") VALUES('"</f>
+        <v xml:space="preserve"> status_id,status_type,status_name,description) VALUES('</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="23" t="str">
+        <f>$C$18&amp;$C$19&amp;C20</f>
+        <v>INSERT INTO tbl_status( status_id,status_type,status_name,description) VALUES('RS01','RS','Waiting,');</v>
+      </c>
+      <c r="C20" s="23" t="str">
+        <f>""&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;","&amp;E5&amp;"');"</f>
+        <v>RS01','RS','Waiting,');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="23" t="str">
+        <f t="shared" ref="A21:A26" si="0">$C$18&amp;$C$19&amp;C21</f>
+        <v>INSERT INTO tbl_status( status_id,status_type,status_name,description) VALUES('RS02','RS','On processing,');</v>
+      </c>
+      <c r="C21" s="23" t="str">
+        <f t="shared" ref="C21:C25" si="1">""&amp;B6&amp;"','"&amp;C6&amp;"','"&amp;D6&amp;","&amp;E6&amp;"');"</f>
+        <v>RS02','RS','On processing,');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_status( status_id,status_type,status_name,description) VALUES('RS03','RS','Cancelled,');</v>
+      </c>
+      <c r="C22" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>RS03','RS','Cancelled,');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_status( status_id,status_type,status_name,description) VALUES('RO01','RO','Not in use,');</v>
+      </c>
+      <c r="C23" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>RO01','RO','Not in use,');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_status( status_id,status_type,status_name,description) VALUES('RO02','RO','In use,');</v>
+      </c>
+      <c r="C24" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>RO02','RO','In use,');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_status( status_id,status_type,status_name,description) VALUES('RO03','RO','Cleaning,');</v>
+      </c>
+      <c r="C25" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>RO03','RO','Cleaning,');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_status( status_id,status_type,status_name,description) VALUES('RO04','RO','Fixing,');</v>
+      </c>
+      <c r="C26" s="23" t="str">
+        <f>""&amp;B11&amp;"','"&amp;C11&amp;"','"&amp;D11&amp;","&amp;E11&amp;"');"</f>
+        <v>RO04','RO','Fixing,');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:J26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="23" customWidth="1"/>
+    <col min="3" max="4" width="9" style="23"/>
+    <col min="5" max="5" width="10.42578125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="10" style="23" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="23" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="23" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="23" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10">
+      <c r="B3" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="1">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" s="23" t="str">
+        <f xml:space="preserve"> "INSERT INTO tbl_reservation("</f>
+        <v>INSERT INTO tbl_reservation(</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19" s="23" t="str">
+        <f>" "&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;") VALUES('"</f>
+        <v xml:space="preserve"> id,status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,create_ymd) VALUES('</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="23" t="str">
+        <f>$C$18&amp;$C$19&amp;C20</f>
+        <v>INSERT INTO tbl_reservation( id,status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,create_ymd) VALUES('1','RS01','','','','','','');</v>
+      </c>
+      <c r="C20" s="23" t="str">
+        <f>""&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"','"&amp;I5&amp;"','"&amp;J5&amp;"');"</f>
+        <v>1','RS01','','','','','','');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="23" t="str">
+        <f t="shared" ref="A21:A26" si="0">$C$18&amp;$C$19&amp;C21</f>
+        <v>INSERT INTO tbl_reservation( id,status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,create_ymd) VALUES('2','RS01','','','','','','');</v>
+      </c>
+      <c r="C21" s="23" t="str">
+        <f>""&amp;B6&amp;"','"&amp;C6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"','"&amp;H6&amp;"','"&amp;I6&amp;"','"&amp;J6&amp;"');"</f>
+        <v>2','RS01','','','','','','');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation( id,status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,create_ymd) VALUES('3','RS01','','','','','','');</v>
+      </c>
+      <c r="C22" s="23" t="str">
+        <f>""&amp;B7&amp;"','"&amp;C7&amp;"','"&amp;E7&amp;"','"&amp;F7&amp;"','"&amp;G7&amp;"','"&amp;H7&amp;"','"&amp;I7&amp;"','"&amp;J7&amp;"');"</f>
+        <v>3','RS01','','','','','','');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation( id,status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,create_ymd) VALUES('4','RS02','','','','','','');</v>
+      </c>
+      <c r="C23" s="23" t="str">
+        <f>""&amp;B8&amp;"','"&amp;C8&amp;"','"&amp;E8&amp;"','"&amp;F8&amp;"','"&amp;G8&amp;"','"&amp;H8&amp;"','"&amp;I8&amp;"','"&amp;J8&amp;"');"</f>
+        <v>4','RS02','','','','','','');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation( id,status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,create_ymd) VALUES('5','RS03','','','','','','');</v>
+      </c>
+      <c r="C24" s="23" t="str">
+        <f>""&amp;B9&amp;"','"&amp;C9&amp;"','"&amp;E9&amp;"','"&amp;F9&amp;"','"&amp;G9&amp;"','"&amp;H9&amp;"','"&amp;I9&amp;"','"&amp;J9&amp;"');"</f>
+        <v>5','RS03','','','','','','');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation( id,status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,create_ymd) VALUES('6','RS03','','','','','','');</v>
+      </c>
+      <c r="C25" s="23" t="str">
+        <f>""&amp;B10&amp;"','"&amp;C10&amp;"','"&amp;E10&amp;"','"&amp;F10&amp;"','"&amp;G10&amp;"','"&amp;H10&amp;"','"&amp;I10&amp;"','"&amp;J10&amp;"');"</f>
+        <v>6','RS03','','','','','','');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tbl_reservation( id,status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,create_ymd) VALUES('7','RS03','','','','','','');</v>
+      </c>
+      <c r="C26" s="23" t="str">
+        <f>""&amp;B11&amp;"','"&amp;C11&amp;"','"&amp;E11&amp;"','"&amp;F11&amp;"','"&amp;G11&amp;"','"&amp;H11&amp;"','"&amp;I11&amp;"','"&amp;J11&amp;"');"</f>
+        <v>7','RS03','','','','','','');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug anh Quyen
</commit_message>
<xml_diff>
--- a/Database/DataSQL-Demo.xlsx
+++ b/Database/DataSQL-Demo.xlsx
@@ -651,36 +651,6 @@
     <t>updater_nm</t>
   </si>
   <si>
-    <t>P101</t>
-  </si>
-  <si>
-    <t>P102</t>
-  </si>
-  <si>
-    <t>P107</t>
-  </si>
-  <si>
-    <t>P108</t>
-  </si>
-  <si>
-    <t>P109</t>
-  </si>
-  <si>
-    <t>P103</t>
-  </si>
-  <si>
-    <t>P104</t>
-  </si>
-  <si>
-    <t>P105</t>
-  </si>
-  <si>
-    <t>P106</t>
-  </si>
-  <si>
-    <t>P110</t>
-  </si>
-  <si>
     <t>P201</t>
   </si>
   <si>
@@ -964,6 +934,36 @@
   </si>
   <si>
     <t>2017/08/24</t>
+  </si>
+  <si>
+    <t>P501</t>
+  </si>
+  <si>
+    <t>P502</t>
+  </si>
+  <si>
+    <t>P503</t>
+  </si>
+  <si>
+    <t>P504</t>
+  </si>
+  <si>
+    <t>P505</t>
+  </si>
+  <si>
+    <t>P506</t>
+  </si>
+  <si>
+    <t>P507</t>
+  </si>
+  <si>
+    <t>P508</t>
+  </si>
+  <si>
+    <t>P509</t>
+  </si>
+  <si>
+    <t>P510</t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1278,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1425,6 +1425,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2105,7 +2106,7 @@
   <dimension ref="A3:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F11"/>
+      <selection activeCell="A20" sqref="A20:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2210,10 +2211,10 @@
         <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>20170825</v>
+        <v>20170831</v>
       </c>
       <c r="F5" s="1">
-        <v>20170829</v>
+        <v>20170902</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
@@ -2244,10 +2245,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="1">
-        <v>20170826</v>
+        <v>20170831</v>
       </c>
       <c r="F6" s="1">
-        <v>20170830</v>
+        <v>20170903</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
@@ -2444,78 +2445,78 @@
     </row>
     <row r="19" spans="1:3">
       <c r="C19" s="23" t="str">
-        <f>" "&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;") VALUES('"</f>
-        <v xml:space="preserve"> status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note) VALUES('</v>
+        <f>" "&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;","&amp;M3&amp;") VALUES('"</f>
+        <v xml:space="preserve"> status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note,editer,update_ymd,create_ymd) VALUES('</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="23" t="str">
         <f>$C$18&amp;$C$19&amp;C20</f>
-        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note) VALUES('RS01','1','20170825','20170829','1','2','0','');</v>
+        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note,editer,update_ymd,create_ymd) VALUES('RS01','1','20170831','20170902','1','2','0','','','2017/08/01','2017/08/01');</v>
       </c>
       <c r="C20" s="23" t="str">
-        <f>""&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"','"&amp;I5&amp;"','"&amp;J5&amp;"');"</f>
-        <v>RS01','1','20170825','20170829','1','2','0','');</v>
+        <f>""&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"','"&amp;I5&amp;"','"&amp;J5&amp;"','"&amp;K5&amp;"','"&amp;L5&amp;"','"&amp;M5&amp;"');"</f>
+        <v>RS01','1','20170831','20170902','1','2','0','','','2017/08/01','2017/08/01');</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="23" t="str">
         <f t="shared" ref="A21:A26" si="0">$C$18&amp;$C$19&amp;C21</f>
-        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note) VALUES('RS01','2','20170826','20170830','2','3','0','');</v>
+        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note,editer,update_ymd,create_ymd) VALUES('RS01','2','20170831','20170903','2','3','0','','','2017/08/02','2017/08/02');</v>
       </c>
       <c r="C21" s="23" t="str">
-        <f t="shared" ref="C21:C26" si="1">""&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"','"&amp;H6&amp;"','"&amp;I6&amp;"','"&amp;J6&amp;"');"</f>
-        <v>RS01','2','20170826','20170830','2','3','0','');</v>
+        <f t="shared" ref="C21:C26" si="1">""&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"','"&amp;H6&amp;"','"&amp;I6&amp;"','"&amp;J6&amp;"','"&amp;K6&amp;"','"&amp;L6&amp;"','"&amp;M6&amp;"');"</f>
+        <v>RS01','2','20170831','20170903','2','3','0','','','2017/08/02','2017/08/02');</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note) VALUES('RS01','3','20170905','20170909','3','4','0','');</v>
+        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note,editer,update_ymd,create_ymd) VALUES('RS01','3','20170905','20170909','3','4','0','','','2017/08/03','2017/08/03');</v>
       </c>
       <c r="C22" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>RS01','3','20170905','20170909','3','4','0','');</v>
+        <v>RS01','3','20170905','20170909','3','4','0','','','2017/08/03','2017/08/03');</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note) VALUES('RS01','4','20170901','20170905','2','3','0','');</v>
+        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note,editer,update_ymd,create_ymd) VALUES('RS01','4','20170901','20170905','2','3','0','','','2017/08/04','2017/08/04');</v>
       </c>
       <c r="C23" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>RS01','4','20170901','20170905','2','3','0','');</v>
+        <v>RS01','4','20170901','20170905','2','3','0','','','2017/08/04','2017/08/04');</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note) VALUES('RS01','5','20170910','20170913','1','1','0','');</v>
+        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note,editer,update_ymd,create_ymd) VALUES('RS01','5','20170910','20170913','1','1','0','','','2017/08/05','2017/08/05');</v>
       </c>
       <c r="C24" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>RS01','5','20170910','20170913','1','1','0','');</v>
+        <v>RS01','5','20170910','20170913','1','1','0','','','2017/08/05','2017/08/05');</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note) VALUES('RS01','6','20170912','20170914','2','2','0','');</v>
+        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note,editer,update_ymd,create_ymd) VALUES('RS01','6','20170912','20170914','2','2','0','','','2017/08/06','2017/08/06');</v>
       </c>
       <c r="C25" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>RS01','6','20170912','20170914','2','2','0','');</v>
+        <v>RS01','6','20170912','20170914','2','2','0','','','2017/08/06','2017/08/06');</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note) VALUES('RS01','7','20170913','20170918','1','2','0','');</v>
+        <v>INSERT INTO tbl_reservation( status_id,guest_id,check_in,check_out,number_of_room,number_of_adult,number_of_children,note,editer,update_ymd,create_ymd) VALUES('RS01','7','20170913','20170918','1','2','0','','','2017/08/07','2017/08/07');</v>
       </c>
       <c r="C26" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>RS01','7','20170913','20170918','1','2','0','');</v>
+        <v>RS01','7','20170913','20170918','1','2','0','','','2017/08/07','2017/08/07');</v>
       </c>
     </row>
   </sheetData>
@@ -2613,13 +2614,13 @@
         <v>139</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="E5" s="33" t="s">
         <v>136</v>
       </c>
       <c r="F5" s="49" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>137</v>
@@ -2642,13 +2643,13 @@
         <v>140</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="E6" s="33" t="s">
         <v>136</v>
       </c>
       <c r="F6" s="49" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>137</v>
@@ -2671,13 +2672,13 @@
         <v>141</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>136</v>
       </c>
       <c r="F7" s="49" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>137</v>
@@ -2700,13 +2701,13 @@
         <v>142</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="E8" s="33" t="s">
         <v>136</v>
       </c>
       <c r="F8" s="49" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>137</v>
@@ -2729,13 +2730,13 @@
         <v>143</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="E9" s="33" t="s">
         <v>136</v>
       </c>
       <c r="F9" s="49" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>137</v>
@@ -2758,13 +2759,13 @@
         <v>113</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="E10" s="33" t="s">
         <v>136</v>
       </c>
       <c r="F10" s="49" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>137</v>
@@ -2787,13 +2788,13 @@
         <v>114</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="E11" s="33" t="s">
         <v>136</v>
       </c>
       <c r="F11" s="49" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>137</v>
@@ -2903,8 +2904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2924,7 +2925,7 @@
     <col min="13" max="16384" width="9" style="23"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="15.75" thickBot="1">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1">
       <c r="B3" s="36" t="s">
         <v>83</v>
       </c>
@@ -2955,7 +2956,7 @@
       <c r="K3" s="50"/>
       <c r="L3" s="51"/>
     </row>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1">
       <c r="B4" s="35" t="s">
         <v>29</v>
       </c>
@@ -2986,8 +2987,8 @@
       <c r="K4" s="50"/>
       <c r="L4" s="51"/>
     </row>
-    <row r="5" spans="2:12">
-      <c r="B5" s="1">
+    <row r="5" spans="1:12">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1">
@@ -3001,18 +3002,18 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="49" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="49" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="J5" s="49"/>
       <c r="K5" s="49"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="2:12">
-      <c r="B6" s="1">
+    <row r="6" spans="1:12">
+      <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="1">
@@ -3026,18 +3027,18 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="49" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="49" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="J6" s="49"/>
       <c r="K6" s="49"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="2:12">
-      <c r="B7" s="1">
+    <row r="7" spans="1:12">
+      <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="C7" s="1">
@@ -3051,18 +3052,18 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="49" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="49" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="J7" s="49"/>
       <c r="K7" s="49"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="2:12">
-      <c r="B8" s="1">
+    <row r="8" spans="1:12">
+      <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="C8" s="1">
@@ -3076,18 +3077,18 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="49" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="49" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="J8" s="49"/>
       <c r="K8" s="49"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="2:12">
-      <c r="B9" s="1">
+    <row r="9" spans="1:12">
+      <c r="A9" s="1">
         <v>5</v>
       </c>
       <c r="C9" s="1">
@@ -3101,18 +3102,18 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="49" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="49" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="J9" s="49"/>
       <c r="K9" s="49"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="2:12">
-      <c r="B10" s="1">
+    <row r="10" spans="1:12">
+      <c r="A10" s="1">
         <v>6</v>
       </c>
       <c r="C10" s="1">
@@ -3126,18 +3127,18 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="49" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="49" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="J10" s="49"/>
       <c r="K10" s="49"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="2:12">
-      <c r="B11" s="1">
+    <row r="11" spans="1:12">
+      <c r="A11" s="1">
         <v>7</v>
       </c>
       <c r="C11" s="1">
@@ -3151,17 +3152,17 @@
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="49" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="49" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="J11" s="49"/>
       <c r="K11" s="49"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="1:12">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -3173,7 +3174,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="1:12">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -3186,7 +3187,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="1:12">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -3199,7 +3200,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="1:12">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -3212,7 +3213,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="1:12">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -3236,84 +3237,84 @@
     </row>
     <row r="24" spans="1:8">
       <c r="C24" s="23" t="str">
-        <f>" "&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;") VALUES('"</f>
-        <v xml:space="preserve"> id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('</v>
+        <f>""&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;") VALUES('"</f>
+        <v>payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1">
       <c r="A25" s="23" t="str">
         <f>$C$23&amp;$C$24&amp;C25</f>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('1','1','1','1','','2017/08/13','','2017/08/13','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('1','1','1','','2017/08/13','','2017/08/13','');</v>
       </c>
       <c r="C25" s="23" t="str">
-        <f>""&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"','"&amp;I5&amp;"','"&amp;J5&amp;"');"</f>
-        <v>1','1','1','1','','2017/08/13','','2017/08/13','');</v>
+        <f>""&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"','"&amp;I5&amp;"','"&amp;J5&amp;"');"</f>
+        <v>1','1','1','','2017/08/13','','2017/08/13','');</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18.75" customHeight="1">
       <c r="A26" s="23" t="str">
         <f t="shared" ref="A26:A39" si="0">$C$23&amp;$C$24&amp;C26</f>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('2','1','2','2','','2017/08/14','','2017/08/14','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('1','2','2','','2017/08/14','','2017/08/14','');</v>
       </c>
       <c r="C26" s="23" t="str">
-        <f t="shared" ref="C26:C31" si="1">""&amp;B6&amp;"','"&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"','"&amp;H6&amp;"','"&amp;I6&amp;"','"&amp;J6&amp;"');"</f>
-        <v>2','1','2','2','','2017/08/14','','2017/08/14','');</v>
+        <f t="shared" ref="C26:C31" si="1">""&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"','"&amp;H6&amp;"','"&amp;I6&amp;"','"&amp;J6&amp;"');"</f>
+        <v>1','2','2','','2017/08/14','','2017/08/14','');</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18.75" customHeight="1">
       <c r="A27" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('3','1','3','3','','2017/08/15','','2017/08/15','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('1','3','3','','2017/08/15','','2017/08/15','');</v>
       </c>
       <c r="C27" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>3','1','3','3','','2017/08/15','','2017/08/15','');</v>
+        <v>1','3','3','','2017/08/15','','2017/08/15','');</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18.75" customHeight="1">
       <c r="A28" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('4','1','4','4','','2017/08/16','','2017/08/16','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('1','4','4','','2017/08/16','','2017/08/16','');</v>
       </c>
       <c r="C28" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>4','1','4','4','','2017/08/16','','2017/08/16','');</v>
+        <v>1','4','4','','2017/08/16','','2017/08/16','');</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18.75" customHeight="1">
       <c r="A29" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('5','1','5','5','','2017/08/17','','2017/08/17','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('1','5','5','','2017/08/17','','2017/08/17','');</v>
       </c>
       <c r="C29" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>5','1','5','5','','2017/08/17','','2017/08/17','');</v>
+        <v>1','5','5','','2017/08/17','','2017/08/17','');</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18.75" customHeight="1">
       <c r="A30" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('6','1','6','6','','2017/08/18','','2017/08/18','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('1','6','6','','2017/08/18','','2017/08/18','');</v>
       </c>
       <c r="C30" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>6','1','6','6','','2017/08/18','','2017/08/18','');</v>
+        <v>1','6','6','','2017/08/18','','2017/08/18','');</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="18.75" customHeight="1">
       <c r="A31" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('7','1','7','7','','2017/08/19','','2017/08/19','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('1','7','7','','2017/08/19','','2017/08/19','');</v>
       </c>
       <c r="C31" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>7','1','7','7','','2017/08/19','','2017/08/19','');</v>
+        <v>1','7','7','','2017/08/19','','2017/08/19','');</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18.75" customHeight="1">
       <c r="A32" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
       </c>
       <c r="C32" s="23" t="str">
         <f t="shared" ref="C32:C39" si="2">""&amp;C12&amp;"','"&amp;D12&amp;"','"&amp;E12&amp;"','"&amp;F12&amp;"','"&amp;G12&amp;"','"&amp;H12&amp;"','"&amp;I12&amp;"','"&amp;J12&amp;"','"&amp;K12&amp;"','"&amp;L12&amp;"');"</f>
@@ -3323,7 +3324,7 @@
     <row r="33" spans="1:3" ht="18.75" customHeight="1">
       <c r="A33" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
       </c>
       <c r="C33" s="23" t="str">
         <f t="shared" si="2"/>
@@ -3333,7 +3334,7 @@
     <row r="34" spans="1:3" ht="18.75" customHeight="1">
       <c r="A34" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
       </c>
       <c r="C34" s="23" t="str">
         <f t="shared" si="2"/>
@@ -3343,7 +3344,7 @@
     <row r="35" spans="1:3" ht="18.75" customHeight="1">
       <c r="A35" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
       </c>
       <c r="C35" s="23" t="str">
         <f t="shared" si="2"/>
@@ -3353,7 +3354,7 @@
     <row r="36" spans="1:3" ht="18.75" customHeight="1">
       <c r="A36" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
       </c>
       <c r="C36" s="23" t="str">
         <f t="shared" si="2"/>
@@ -3363,7 +3364,7 @@
     <row r="37" spans="1:3" ht="18.75" customHeight="1">
       <c r="A37" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
       </c>
       <c r="C37" s="23" t="str">
         <f t="shared" si="2"/>
@@ -3373,7 +3374,7 @@
     <row r="38" spans="1:3" ht="18.75" customHeight="1">
       <c r="A38" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
       </c>
       <c r="C38" s="23" t="str">
         <f t="shared" si="2"/>
@@ -3383,7 +3384,7 @@
     <row r="39" spans="1:3" ht="18.75" customHeight="1">
       <c r="A39" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_invoice( id,payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
+        <v>INSERT INTO tbl_invoice(payment_type_id,reservation_id,guest_id,tax_code,update_ymd,updater_nm,create_ymd,creater_nm) VALUES('','','','','','','','','','');</v>
       </c>
       <c r="C39" s="23" t="str">
         <f t="shared" si="2"/>
@@ -3400,8 +3401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:A36"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3432,10 +3433,10 @@
         <v>157</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="F3" s="50" t="s">
         <v>158</v>
@@ -3521,7 +3522,7 @@
         <v>129</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -3538,13 +3539,13 @@
         <v>129</v>
       </c>
       <c r="K5" s="49" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="N5" s="49" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="O5" s="49" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -3556,7 +3557,7 @@
         <v>130</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -3573,13 +3574,13 @@
         <v>130</v>
       </c>
       <c r="K6" s="49" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="N6" s="49" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="O6" s="49" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="2:15">
@@ -3591,7 +3592,7 @@
         <v>131</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -3608,13 +3609,13 @@
         <v>131</v>
       </c>
       <c r="K7" s="49" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="N7" s="49" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="O7" s="49" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="2:15">
@@ -3626,7 +3627,7 @@
         <v>129</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -3643,13 +3644,13 @@
         <v>129</v>
       </c>
       <c r="K8" s="49" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="N8" s="49" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="O8" s="49" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="2:15">
@@ -3661,7 +3662,7 @@
         <v>130</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -3678,13 +3679,13 @@
         <v>130</v>
       </c>
       <c r="K9" s="49" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="N9" s="49" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="O9" s="49" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="2:15">
@@ -3696,7 +3697,7 @@
         <v>131</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -3713,13 +3714,13 @@
         <v>131</v>
       </c>
       <c r="K10" s="49" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="N10" s="49" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="O10" s="49" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="2:15">
@@ -3731,7 +3732,7 @@
         <v>132</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -3748,13 +3749,13 @@
         <v>132</v>
       </c>
       <c r="K11" s="49" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="N11" s="49" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="O11" s="49" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="2:15">
@@ -3766,7 +3767,7 @@
         <v>133</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
@@ -3783,13 +3784,13 @@
         <v>133</v>
       </c>
       <c r="K12" s="49" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="N12" s="49" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="O12" s="49" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="2:15">
@@ -3801,7 +3802,7 @@
         <v>129</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -3818,13 +3819,13 @@
         <v>129</v>
       </c>
       <c r="K13" s="49" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="N13" s="49" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="O13" s="49" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="2:15">
@@ -3836,7 +3837,7 @@
         <v>130</v>
       </c>
       <c r="E14" s="53" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -3853,13 +3854,13 @@
         <v>130</v>
       </c>
       <c r="K14" s="49" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="N14" s="49" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="O14" s="49" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="2:15">
@@ -3871,7 +3872,7 @@
         <v>131</v>
       </c>
       <c r="E15" s="53" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
@@ -3888,13 +3889,13 @@
         <v>131</v>
       </c>
       <c r="K15" s="49" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="N15" s="49" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="O15" s="49" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="2:15">
@@ -3906,7 +3907,7 @@
         <v>132</v>
       </c>
       <c r="E16" s="53" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -3923,13 +3924,13 @@
         <v>132</v>
       </c>
       <c r="K16" s="49" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="N16" s="49" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="O16" s="49" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3950,147 +3951,147 @@
         <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('1','RO001','Room','1','400000','','440000','RO001','1','','','2017/08/13','2017/08/13');</v>
       </c>
       <c r="C25" s="23" t="str">
-        <f>""&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"','"&amp;I5&amp;"','"&amp;J5&amp;"','"&amp;K5&amp;"','"&amp;L5&amp;"','"&amp;M5&amp;"','"&amp;N5&amp;"','"&amp;O5&amp;"');"</f>
+        <f t="shared" ref="C25:C36" si="1">""&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"','"&amp;I5&amp;"','"&amp;J5&amp;"','"&amp;K5&amp;"','"&amp;L5&amp;"','"&amp;M5&amp;"','"&amp;N5&amp;"','"&amp;O5&amp;"');"</f>
         <v>1','RO001','Room','1','400000','','440000','RO001','1','','','2017/08/13','2017/08/13');</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="23" t="str">
-        <f t="shared" ref="A26:A39" si="1">$C$23&amp;$C$24&amp;C26</f>
+        <f t="shared" ref="A26:A39" si="2">$C$23&amp;$C$24&amp;C26</f>
         <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('2','RO002','Room','1','400000','','440000','RO002','1','','','2017/08/14','2017/08/14');</v>
       </c>
       <c r="C26" s="23" t="str">
-        <f>""&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"','"&amp;H6&amp;"','"&amp;I6&amp;"','"&amp;J6&amp;"','"&amp;K6&amp;"','"&amp;L6&amp;"','"&amp;M6&amp;"','"&amp;N6&amp;"','"&amp;O6&amp;"');"</f>
+        <f t="shared" si="1"/>
         <v>2','RO002','Room','1','400000','','440000','RO002','1','','','2017/08/14','2017/08/14');</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('2','RO003','Room','1','400000','','440000','RO003','1','','','2017/08/15','2017/08/15');</v>
+      </c>
+      <c r="C27" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('2','RO003','Room','1','400000','','440000','RO003','1','','','2017/08/15','2017/08/15');</v>
-      </c>
-      <c r="C27" s="23" t="str">
-        <f>""&amp;C7&amp;"','"&amp;D7&amp;"','"&amp;E7&amp;"','"&amp;F7&amp;"','"&amp;G7&amp;"','"&amp;H7&amp;"','"&amp;I7&amp;"','"&amp;J7&amp;"','"&amp;K7&amp;"','"&amp;L7&amp;"','"&amp;M7&amp;"','"&amp;N7&amp;"','"&amp;O7&amp;"');"</f>
         <v>2','RO003','Room','1','400000','','440000','RO003','1','','','2017/08/15','2017/08/15');</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('3','RO001','Room','1','400000','','440000','RO001','1','','','2017/08/16','2017/08/16');</v>
+      </c>
+      <c r="C28" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('3','RO001','Room','1','400000','','440000','RO001','1','','','2017/08/16','2017/08/16');</v>
-      </c>
-      <c r="C28" s="23" t="str">
-        <f>""&amp;C8&amp;"','"&amp;D8&amp;"','"&amp;E8&amp;"','"&amp;F8&amp;"','"&amp;G8&amp;"','"&amp;H8&amp;"','"&amp;I8&amp;"','"&amp;J8&amp;"','"&amp;K8&amp;"','"&amp;L8&amp;"','"&amp;M8&amp;"','"&amp;N8&amp;"','"&amp;O8&amp;"');"</f>
         <v>3','RO001','Room','1','400000','','440000','RO001','1','','','2017/08/16','2017/08/16');</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('3','RO002','Room','1','400000','','440000','RO002','1','','','2017/08/17','2017/08/17');</v>
+      </c>
+      <c r="C29" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('3','RO002','Room','1','400000','','440000','RO002','1','','','2017/08/17','2017/08/17');</v>
-      </c>
-      <c r="C29" s="23" t="str">
-        <f>""&amp;C9&amp;"','"&amp;D9&amp;"','"&amp;E9&amp;"','"&amp;F9&amp;"','"&amp;G9&amp;"','"&amp;H9&amp;"','"&amp;I9&amp;"','"&amp;J9&amp;"','"&amp;K9&amp;"','"&amp;L9&amp;"','"&amp;M9&amp;"','"&amp;N9&amp;"','"&amp;O9&amp;"');"</f>
         <v>3','RO002','Room','1','400000','','440000','RO002','1','','','2017/08/17','2017/08/17');</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('3','RO003','Room','1','400000','','440000','RO003','1','','','2017/08/18','2017/08/18');</v>
+      </c>
+      <c r="C30" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('3','RO003','Room','1','400000','','440000','RO003','1','','','2017/08/18','2017/08/18');</v>
-      </c>
-      <c r="C30" s="23" t="str">
-        <f>""&amp;C10&amp;"','"&amp;D10&amp;"','"&amp;E10&amp;"','"&amp;F10&amp;"','"&amp;G10&amp;"','"&amp;H10&amp;"','"&amp;I10&amp;"','"&amp;J10&amp;"','"&amp;K10&amp;"','"&amp;L10&amp;"','"&amp;M10&amp;"','"&amp;N10&amp;"','"&amp;O10&amp;"');"</f>
         <v>3','RO003','Room','1','400000','','440000','RO003','1','','','2017/08/18','2017/08/18');</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('4','RO004','Room','1','400000','','440000','RO004','1','','','2017/08/19','2017/08/19');</v>
+      </c>
+      <c r="C31" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('4','RO004','Room','1','400000','','440000','RO004','1','','','2017/08/19','2017/08/19');</v>
-      </c>
-      <c r="C31" s="23" t="str">
-        <f>""&amp;C11&amp;"','"&amp;D11&amp;"','"&amp;E11&amp;"','"&amp;F11&amp;"','"&amp;G11&amp;"','"&amp;H11&amp;"','"&amp;I11&amp;"','"&amp;J11&amp;"','"&amp;K11&amp;"','"&amp;L11&amp;"','"&amp;M11&amp;"','"&amp;N11&amp;"','"&amp;O11&amp;"');"</f>
         <v>4','RO004','Room','1','400000','','440000','RO004','1','','','2017/08/19','2017/08/19');</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('4','RO005','Room','1','400000','','440000','RO005','1','','','2017/08/20','2017/08/20');</v>
+      </c>
+      <c r="C32" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('4','RO005','Room','1','400000','','440000','RO005','1','','','2017/08/20','2017/08/20');</v>
-      </c>
-      <c r="C32" s="23" t="str">
-        <f>""&amp;C12&amp;"','"&amp;D12&amp;"','"&amp;E12&amp;"','"&amp;F12&amp;"','"&amp;G12&amp;"','"&amp;H12&amp;"','"&amp;I12&amp;"','"&amp;J12&amp;"','"&amp;K12&amp;"','"&amp;L12&amp;"','"&amp;M12&amp;"','"&amp;N12&amp;"','"&amp;O12&amp;"');"</f>
         <v>4','RO005','Room','1','400000','','440000','RO005','1','','','2017/08/20','2017/08/20');</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('5','RO001','Room','1','300000','','330000','RO001','1','','','2017/08/21','2017/08/21');</v>
+      </c>
+      <c r="C33" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('5','RO001','Room','1','300000','','330000','RO001','1','','','2017/08/21','2017/08/21');</v>
-      </c>
-      <c r="C33" s="23" t="str">
-        <f>""&amp;C13&amp;"','"&amp;D13&amp;"','"&amp;E13&amp;"','"&amp;F13&amp;"','"&amp;G13&amp;"','"&amp;H13&amp;"','"&amp;I13&amp;"','"&amp;J13&amp;"','"&amp;K13&amp;"','"&amp;L13&amp;"','"&amp;M13&amp;"','"&amp;N13&amp;"','"&amp;O13&amp;"');"</f>
         <v>5','RO001','Room','1','300000','','330000','RO001','1','','','2017/08/21','2017/08/21');</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('6','RO002','Room','1','200000','','220000','RO002','1','','','2017/08/22','2017/08/22');</v>
+      </c>
+      <c r="C34" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('6','RO002','Room','1','200000','','220000','RO002','1','','','2017/08/22','2017/08/22');</v>
-      </c>
-      <c r="C34" s="23" t="str">
-        <f>""&amp;C14&amp;"','"&amp;D14&amp;"','"&amp;E14&amp;"','"&amp;F14&amp;"','"&amp;G14&amp;"','"&amp;H14&amp;"','"&amp;I14&amp;"','"&amp;J14&amp;"','"&amp;K14&amp;"','"&amp;L14&amp;"','"&amp;M14&amp;"','"&amp;N14&amp;"','"&amp;O14&amp;"');"</f>
         <v>6','RO002','Room','1','200000','','220000','RO002','1','','','2017/08/22','2017/08/22');</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('6','RO003','Room','1','200000','','220000','RO003','1','','','2017/08/23','2017/08/23');</v>
+      </c>
+      <c r="C35" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('6','RO003','Room','1','200000','','220000','RO003','1','','','2017/08/23','2017/08/23');</v>
-      </c>
-      <c r="C35" s="23" t="str">
-        <f>""&amp;C15&amp;"','"&amp;D15&amp;"','"&amp;E15&amp;"','"&amp;F15&amp;"','"&amp;G15&amp;"','"&amp;H15&amp;"','"&amp;I15&amp;"','"&amp;J15&amp;"','"&amp;K15&amp;"','"&amp;L15&amp;"','"&amp;M15&amp;"','"&amp;N15&amp;"','"&amp;O15&amp;"');"</f>
         <v>6','RO003','Room','1','200000','','220000','RO003','1','','','2017/08/23','2017/08/23');</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('7','RO004','Room','1','500000','','550000','RO004','1','','','2017/08/24','2017/08/24');</v>
+      </c>
+      <c r="C36" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('7','RO004','Room','1','500000','','550000','RO004','1','','','2017/08/24','2017/08/24');</v>
-      </c>
-      <c r="C36" s="23" t="str">
-        <f>""&amp;C16&amp;"','"&amp;D16&amp;"','"&amp;E16&amp;"','"&amp;F16&amp;"','"&amp;G16&amp;"','"&amp;H16&amp;"','"&amp;I16&amp;"','"&amp;J16&amp;"','"&amp;K16&amp;"','"&amp;L16&amp;"','"&amp;M16&amp;"','"&amp;N16&amp;"','"&amp;O16&amp;"');"</f>
         <v>7','RO004','Room','1','500000','','550000','RO004','1','','','2017/08/24','2017/08/24');</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('','','','','','','','','');</v>
       </c>
       <c r="C37" s="23" t="str">
-        <f t="shared" ref="C37:C39" si="2">""&amp;C17&amp;"','"&amp;D17&amp;"','"&amp;E17&amp;"','"&amp;F17&amp;"','"&amp;G17&amp;"','"&amp;H17&amp;"','"&amp;I17&amp;"','"&amp;J17&amp;"','"&amp;K17&amp;"');"</f>
+        <f t="shared" ref="C37:C39" si="3">""&amp;C17&amp;"','"&amp;D17&amp;"','"&amp;E17&amp;"','"&amp;F17&amp;"','"&amp;G17&amp;"','"&amp;H17&amp;"','"&amp;I17&amp;"','"&amp;J17&amp;"','"&amp;K17&amp;"');"</f>
         <v>','','','','','','','','');</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('','','','','','','','','');</v>
       </c>
       <c r="C38" s="23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>','','','','','','','','');</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO tbl_invoice_detail( invoice_id,item_id,item_type,quantity,price,description,amount_total,room_id,payment_flag,creater_nm,updater_nm,update_ymd,create_ymd) VALUES('','','','','','','','','');</v>
       </c>
       <c r="C39" s="23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>','','','','','','','','');</v>
       </c>
     </row>
@@ -5413,16 +5414,16 @@
         <v>74</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="F3" s="36" t="s">
         <v>75</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="H3" s="37" t="s">
         <v>76</v>
@@ -5480,16 +5481,16 @@
         <v>195</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="H5" s="1">
         <v>400000</v>
       </c>
       <c r="I5" s="59" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="J5" s="59" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="2:10">
@@ -5509,16 +5510,16 @@
         <v>198</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="H6" s="1">
         <v>600000</v>
       </c>
       <c r="I6" s="59" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="J6" s="59" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="2:10">
@@ -5538,16 +5539,16 @@
         <v>196</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="H7" s="1">
         <v>700000</v>
       </c>
       <c r="I7" s="59" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="J7" s="59" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="2:10">
@@ -5567,16 +5568,16 @@
         <v>197</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="H8" s="1">
         <v>900000</v>
       </c>
       <c r="I8" s="59" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="J8" s="59" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="2:10">
@@ -5708,7 +5709,7 @@
         <v>118</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -5720,7 +5721,7 @@
         <v>118</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -5732,7 +5733,7 @@
         <v>118</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -5744,7 +5745,7 @@
         <v>118</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -5756,7 +5757,7 @@
         <v>118</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -5768,7 +5769,7 @@
         <v>119</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -5780,7 +5781,7 @@
         <v>119</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -5792,7 +5793,7 @@
         <v>119</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -5804,7 +5805,7 @@
         <v>119</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -5920,7 +5921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="A49" sqref="A49:A88"/>
     </sheetView>
   </sheetViews>
@@ -5980,7 +5981,7 @@
         <v>125</v>
       </c>
       <c r="E5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>120</v>
@@ -5998,7 +5999,7 @@
         <v>125</v>
       </c>
       <c r="E6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>120</v>
@@ -6016,13 +6017,13 @@
         <v>125</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="2:7">
@@ -6034,13 +6035,13 @@
         <v>125</v>
       </c>
       <c r="E8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="2:7">
@@ -6052,13 +6053,13 @@
         <v>125</v>
       </c>
       <c r="E9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="2:7">
@@ -6070,13 +6071,13 @@
         <v>125</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="2:7">
@@ -6088,13 +6089,13 @@
         <v>125</v>
       </c>
       <c r="E11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="2:7">
@@ -6106,13 +6107,13 @@
         <v>125</v>
       </c>
       <c r="E12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="2:7">
@@ -6124,13 +6125,13 @@
         <v>125</v>
       </c>
       <c r="E13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="2:7">
@@ -6142,7 +6143,7 @@
         <v>125</v>
       </c>
       <c r="E14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>120</v>
@@ -6160,13 +6161,13 @@
         <v>126</v>
       </c>
       <c r="E15" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>211</v>
+      <c r="G15" s="34" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="2:7">
@@ -6178,13 +6179,13 @@
         <v>126</v>
       </c>
       <c r="E16" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>212</v>
+      <c r="G16" s="34" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="3:7">
@@ -6195,13 +6196,13 @@
         <v>126</v>
       </c>
       <c r="E17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>217</v>
+      <c r="G17" s="34" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="3:7">
@@ -6212,13 +6213,13 @@
         <v>126</v>
       </c>
       <c r="E18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>218</v>
+      <c r="G18" s="34" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="3:7">
@@ -6229,13 +6230,13 @@
         <v>126</v>
       </c>
       <c r="E19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>219</v>
+      <c r="G19" s="34" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="3:7">
@@ -6246,13 +6247,13 @@
         <v>126</v>
       </c>
       <c r="E20" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>213</v>
+      <c r="G20" s="34" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="3:7">
@@ -6263,13 +6264,13 @@
         <v>126</v>
       </c>
       <c r="E21" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>214</v>
+      <c r="G21" s="34" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="3:7">
@@ -6280,13 +6281,13 @@
         <v>126</v>
       </c>
       <c r="E22" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>215</v>
+      <c r="G22" s="34" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="3:7">
@@ -6297,13 +6298,13 @@
         <v>126</v>
       </c>
       <c r="E23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>216</v>
+      <c r="G23" s="34" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="3:7">
@@ -6314,13 +6315,13 @@
         <v>126</v>
       </c>
       <c r="E24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>220</v>
+      <c r="G24" s="34" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="3:7">
@@ -6331,340 +6332,341 @@
         <v>127</v>
       </c>
       <c r="E25" s="34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G25" s="34" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="3:7" ht="16.5" customHeight="1">
       <c r="C26" s="1" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D26" s="34" t="s">
         <v>127</v>
       </c>
       <c r="E26" s="34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="3:7" ht="16.5" customHeight="1">
       <c r="C27" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="D27" s="34" t="s">
         <v>127</v>
       </c>
       <c r="E27" s="34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="3:7" ht="16.5" customHeight="1">
       <c r="C28" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D28" s="34" t="s">
         <v>127</v>
       </c>
       <c r="E28" s="34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="3:7" ht="16.5" customHeight="1">
       <c r="C29" s="1" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D29" s="34" t="s">
         <v>127</v>
       </c>
       <c r="E29" s="34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="3:7" ht="16.5" customHeight="1">
       <c r="C30" s="1" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D30" s="34" t="s">
         <v>127</v>
       </c>
       <c r="E30" s="34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G30" s="34" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="3:7" ht="16.5" customHeight="1">
       <c r="C31" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D31" s="34" t="s">
         <v>127</v>
       </c>
       <c r="E31" s="34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G31" s="34" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="3:7" ht="16.5" customHeight="1">
       <c r="C32" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D32" s="34" t="s">
         <v>127</v>
       </c>
       <c r="E32" s="34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33" spans="3:7" ht="16.5" customHeight="1">
       <c r="C33" s="1" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D33" s="34" t="s">
         <v>127</v>
       </c>
       <c r="E33" s="34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G33" s="34" t="s">
-        <v>231</v>
+        <v>248</v>
       </c>
     </row>
     <row r="34" spans="3:7" ht="16.5" customHeight="1">
       <c r="C34" s="1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D34" s="34" t="s">
         <v>127</v>
       </c>
       <c r="E34" s="34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G34" s="34" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="3:7" ht="16.5" customHeight="1">
       <c r="C35" s="1" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D35" s="34" t="s">
         <v>128</v>
       </c>
       <c r="E35" s="34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G35" s="34" t="s">
-        <v>250</v>
+        <v>296</v>
       </c>
     </row>
     <row r="36" spans="3:7">
       <c r="C36" s="1" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D36" s="34" t="s">
         <v>128</v>
       </c>
       <c r="E36" s="34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>251</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="3:7">
       <c r="C37" s="1" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D37" s="34" t="s">
         <v>128</v>
       </c>
       <c r="E37" s="34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>252</v>
+        <v>298</v>
       </c>
     </row>
     <row r="38" spans="3:7">
       <c r="C38" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D38" s="34" t="s">
         <v>128</v>
       </c>
       <c r="E38" s="34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G38" s="34" t="s">
-        <v>253</v>
+        <v>299</v>
       </c>
     </row>
     <row r="39" spans="3:7">
       <c r="C39" s="1" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D39" s="34" t="s">
         <v>128</v>
       </c>
       <c r="E39" s="34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>254</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="3:7">
       <c r="C40" s="1" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D40" s="34" t="s">
         <v>128</v>
       </c>
       <c r="E40" s="34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>255</v>
+        <v>301</v>
       </c>
     </row>
     <row r="41" spans="3:7">
       <c r="C41" s="1" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="D41" s="34" t="s">
         <v>128</v>
       </c>
       <c r="E41" s="34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>256</v>
+        <v>302</v>
       </c>
     </row>
     <row r="42" spans="3:7">
       <c r="C42" s="1" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="D42" s="34" t="s">
         <v>128</v>
       </c>
       <c r="E42" s="34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G42" s="34" t="s">
-        <v>257</v>
+        <v>303</v>
       </c>
     </row>
     <row r="43" spans="3:7">
       <c r="C43" s="1" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D43" s="34" t="s">
         <v>128</v>
       </c>
       <c r="E43" s="34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G43" s="34" t="s">
-        <v>258</v>
+        <v>304</v>
       </c>
     </row>
     <row r="44" spans="3:7">
       <c r="C44" s="1" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="D44" s="34" t="s">
         <v>128</v>
       </c>
       <c r="E44" s="34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>120</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>259</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45" spans="3:7">
       <c r="C45" s="19"/>
+      <c r="G45" s="60"/>
     </row>
     <row r="47" spans="3:7">
       <c r="C47" s="23" t="str">
@@ -6678,404 +6680,404 @@
         <v xml:space="preserve"> room_id,room_type_id,floor,status_id,room_number) VALUES('</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1">
+    <row r="49" spans="1:3" ht="18.75" customHeight="1">
       <c r="A49" s="23" t="str">
         <f>$C$47&amp;$C$48&amp;C49</f>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO001','RT01','1','RO01','P101');</v>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO001','RT01','2','RO01','P201');</v>
       </c>
       <c r="C49" s="23" t="str">
         <f>""&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"');"</f>
-        <v>RO001','RT01','1','RO01','P101');</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO001','RT01','2','RO01','P201');</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="18.75" customHeight="1">
       <c r="A50" s="23" t="str">
-        <f t="shared" ref="A50:A56" si="0">$C$47&amp;$C$48&amp;C50</f>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO002','RT01','1','RO01','P102');</v>
+        <f t="shared" ref="A50:A58" si="0">$C$47&amp;$C$48&amp;C50</f>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO002','RT01','2','RO01','P202');</v>
       </c>
       <c r="C50" s="23" t="str">
-        <f t="shared" ref="C50:C88" si="1">""&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"');"</f>
-        <v>RO002','RT01','1','RO01','P102');</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" ref="C50:C58" si="1">""&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"');"</f>
+        <v>RO002','RT01','2','RO01','P202');</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="18.75" customHeight="1">
       <c r="A51" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO003','RT01','1','RO01','P103');</v>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO003','RT01','2','RO01','P203');</v>
       </c>
       <c r="C51" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>RO003','RT01','1','RO01','P103');</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO003','RT01','2','RO01','P203');</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="18.75" customHeight="1">
       <c r="A52" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO004','RT01','1','RO01','P104');</v>
+        <f t="shared" ref="A52:A88" si="2">$C$47&amp;$C$48&amp;C52</f>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO004','RT01','2','RO01','P204');</v>
       </c>
       <c r="C52" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO004','RT01','1','RO01','P104');</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" ref="C52:C88" si="3">""&amp;C8&amp;"','"&amp;D8&amp;"','"&amp;E8&amp;"','"&amp;F8&amp;"','"&amp;G8&amp;"');"</f>
+        <v>RO004','RT01','2','RO01','P204');</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="18.75" customHeight="1">
       <c r="A53" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO005','RT01','1','RO01','P105');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO005','RT01','2','RO01','P205');</v>
       </c>
       <c r="C53" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO005','RT01','1','RO01','P105');</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO005','RT01','2','RO01','P205');</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="18.75" customHeight="1">
       <c r="A54" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO006','RT01','1','RO01','P106');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO006','RT01','2','RO01','P206');</v>
       </c>
       <c r="C54" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO006','RT01','1','RO01','P106');</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO006','RT01','2','RO01','P206');</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="18.75" customHeight="1">
       <c r="A55" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO007','RT01','1','RO01','P107');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO007','RT01','2','RO01','P207');</v>
       </c>
       <c r="C55" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO007','RT01','1','RO01','P107');</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO007','RT01','2','RO01','P207');</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="18.75" customHeight="1">
       <c r="A56" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO008','RT01','1','RO01','P108');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO008','RT01','2','RO01','P208');</v>
       </c>
       <c r="C56" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO008','RT01','1','RO01','P108');</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO008','RT01','2','RO01','P208');</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="18.75" customHeight="1">
       <c r="A57" s="23" t="str">
-        <f t="shared" ref="A57:A65" si="2">$C$47&amp;$C$48&amp;C57</f>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO009','RT01','1','RO01','P109');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO009','RT01','2','RO01','P209');</v>
       </c>
       <c r="C57" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO009','RT01','1','RO01','P109');</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO009','RT01','2','RO01','P209');</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="18.75" customHeight="1">
       <c r="A58" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO010','RT01','1','RO01','P110');</v>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO010','RT01','2','RO01','P210');</v>
       </c>
       <c r="C58" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO010','RT01','1','RO01','P110');</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO010','RT01','2','RO01','P210');</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="18.75" customHeight="1">
       <c r="A59" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO011','RT02','2','RO01','P201');</v>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO011','RT02','3','RO01','P301');</v>
       </c>
       <c r="C59" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO011','RT02','2','RO01','P201');</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO011','RT02','3','RO01','P301');</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="18.75" customHeight="1">
       <c r="A60" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO012','RT02','2','RO01','P202');</v>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO012','RT02','3','RO01','P302');</v>
       </c>
       <c r="C60" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO012','RT02','2','RO01','P202');</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO012','RT02','3','RO01','P302');</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="18.75" customHeight="1">
       <c r="A61" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO013','RT02','2','RO01','P203');</v>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO013','RT02','3','RO01','P303');</v>
       </c>
       <c r="C61" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO013','RT02','2','RO01','P203');</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO013','RT02','3','RO01','P303');</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="18.75" customHeight="1">
       <c r="A62" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO014','RT02','2','RO01','P204');</v>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO014','RT02','3','RO01','P304');</v>
       </c>
       <c r="C62" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO014','RT02','2','RO01','P204');</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO014','RT02','3','RO01','P304');</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="18.75" customHeight="1">
       <c r="A63" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO015','RT02','2','RO01','P205');</v>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO015','RT02','3','RO01','P305');</v>
       </c>
       <c r="C63" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO015','RT02','2','RO01','P205');</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO015','RT02','3','RO01','P305');</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="18.75" customHeight="1">
       <c r="A64" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO016','RT02','2','RO01','P206');</v>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO016','RT02','3','RO01','P306');</v>
       </c>
       <c r="C64" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO016','RT02','2','RO01','P206');</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO016','RT02','3','RO01','P306');</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="18.75" customHeight="1">
       <c r="A65" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO017','RT02','2','RO01','P207');</v>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO017','RT02','3','RO01','P307');</v>
       </c>
       <c r="C65" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO017','RT02','2','RO01','P207');</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO017','RT02','3','RO01','P307');</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="18.75" customHeight="1">
       <c r="A66" s="23" t="str">
-        <f t="shared" ref="A66:A88" si="3">$C$47&amp;$C$48&amp;C66</f>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO018','RT02','2','RO01','P208');</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO018','RT02','3','RO01','P308');</v>
       </c>
       <c r="C66" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO018','RT02','2','RO01','P208');</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1">
+        <f t="shared" si="3"/>
+        <v>RO018','RT02','3','RO01','P308');</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="18.75" customHeight="1">
       <c r="A67" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO019','RT02','3','RO01','P309');</v>
+      </c>
+      <c r="C67" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO019','RT02','2','RO01','P209');</v>
-      </c>
-      <c r="C67" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO019','RT02','2','RO01','P209');</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO019','RT02','3','RO01','P309');</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="18.75" customHeight="1">
       <c r="A68" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO020','RT02','3','RO01','P310');</v>
+      </c>
+      <c r="C68" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO020','RT02','2','RO01','P210');</v>
-      </c>
-      <c r="C68" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO020','RT02','2','RO01','P210');</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO020','RT02','3','RO01','P310');</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="18.75" customHeight="1">
       <c r="A69" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO021','RT03','4','RO01','P401');</v>
+      </c>
+      <c r="C69" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO021','RT03','3','RO01','P301');</v>
-      </c>
-      <c r="C69" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO021','RT03','3','RO01','P301');</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO021','RT03','4','RO01','P401');</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="18.75" customHeight="1">
       <c r="A70" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO022','RT03','4','RO01','P402');</v>
+      </c>
+      <c r="C70" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO022','RT03','3','RO01','P302');</v>
-      </c>
-      <c r="C70" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO022','RT03','3','RO01','P302');</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO022','RT03','4','RO01','P402');</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="18.75" customHeight="1">
       <c r="A71" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO023','RT03','4','RO01','P403');</v>
+      </c>
+      <c r="C71" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO023','RT03','3','RO01','P303');</v>
-      </c>
-      <c r="C71" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO023','RT03','3','RO01','P303');</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO023','RT03','4','RO01','P403');</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="18.75" customHeight="1">
       <c r="A72" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO024','RT03','4','RO01','P404');</v>
+      </c>
+      <c r="C72" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO024','RT03','3','RO01','P304');</v>
-      </c>
-      <c r="C72" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO024','RT03','3','RO01','P304');</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO024','RT03','4','RO01','P404');</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="18.75" customHeight="1">
       <c r="A73" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO025','RT03','4','RO01','P405');</v>
+      </c>
+      <c r="C73" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO025','RT03','3','RO01','P305');</v>
-      </c>
-      <c r="C73" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO025','RT03','3','RO01','P305');</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO025','RT03','4','RO01','P405');</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="18.75" customHeight="1">
       <c r="A74" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO026','RT03','4','RO01','P406');</v>
+      </c>
+      <c r="C74" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO026','RT03','3','RO01','P306');</v>
-      </c>
-      <c r="C74" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO026','RT03','3','RO01','P306');</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO026','RT03','4','RO01','P406');</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="18.75" customHeight="1">
       <c r="A75" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO027','RT03','4','RO01','P407');</v>
+      </c>
+      <c r="C75" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO027','RT03','3','RO01','P307');</v>
-      </c>
-      <c r="C75" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO027','RT03','3','RO01','P307');</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO027','RT03','4','RO01','P407');</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="18.75" customHeight="1">
       <c r="A76" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO028','RT03','4','RO01','P408');</v>
+      </c>
+      <c r="C76" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO028','RT03','3','RO01','P308');</v>
-      </c>
-      <c r="C76" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO028','RT03','3','RO01','P308');</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO028','RT03','4','RO01','P408');</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="18.75" customHeight="1">
       <c r="A77" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO029','RT03','4','RO01','P409');</v>
+      </c>
+      <c r="C77" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO029','RT03','3','RO01','P309');</v>
-      </c>
-      <c r="C77" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO029','RT03','3','RO01','P309');</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO029','RT03','4','RO01','P409');</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="18.75" customHeight="1">
       <c r="A78" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO030','RT03','4','RO01','P410');</v>
+      </c>
+      <c r="C78" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO030','RT03','3','RO01','P310');</v>
-      </c>
-      <c r="C78" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO030','RT03','3','RO01','P310');</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO030','RT03','4','RO01','P410');</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="18.75" customHeight="1">
       <c r="A79" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO031','RT04','5','RO01','P501');</v>
+      </c>
+      <c r="C79" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO031','RT04','4','RO01','P401');</v>
-      </c>
-      <c r="C79" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO031','RT04','4','RO01','P401');</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO031','RT04','5','RO01','P501');</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="18.75" customHeight="1">
       <c r="A80" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO032','RT04','5','RO01','P502');</v>
+      </c>
+      <c r="C80" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO032','RT04','4','RO01','P402');</v>
-      </c>
-      <c r="C80" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO032','RT04','4','RO01','P402');</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO032','RT04','5','RO01','P502');</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="18.75" customHeight="1">
       <c r="A81" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO033','RT04','5','RO01','P503');</v>
+      </c>
+      <c r="C81" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO033','RT04','4','RO01','P403');</v>
-      </c>
-      <c r="C81" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO033','RT04','4','RO01','P403');</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO033','RT04','5','RO01','P503');</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="18.75" customHeight="1">
       <c r="A82" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO034','RT04','5','RO01','P504');</v>
+      </c>
+      <c r="C82" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO034','RT04','4','RO01','P404');</v>
-      </c>
-      <c r="C82" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO034','RT04','4','RO01','P404');</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO034','RT04','5','RO01','P504');</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="18.75" customHeight="1">
       <c r="A83" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO035','RT04','5','RO01','P505');</v>
+      </c>
+      <c r="C83" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO035','RT04','4','RO01','P405');</v>
-      </c>
-      <c r="C83" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO035','RT04','4','RO01','P405');</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO035','RT04','5','RO01','P505');</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="18.75" customHeight="1">
       <c r="A84" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO036','RT04','5','RO01','P506');</v>
+      </c>
+      <c r="C84" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO036','RT04','4','RO01','P406');</v>
-      </c>
-      <c r="C84" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO036','RT04','4','RO01','P406');</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO036','RT04','5','RO01','P506');</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="18.75" customHeight="1">
       <c r="A85" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO037','RT04','5','RO01','P507');</v>
+      </c>
+      <c r="C85" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO037','RT04','4','RO01','P407');</v>
-      </c>
-      <c r="C85" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO037','RT04','4','RO01','P407');</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO037','RT04','5','RO01','P507');</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="18.75" customHeight="1">
       <c r="A86" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO038','RT04','5','RO01','P508');</v>
+      </c>
+      <c r="C86" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO038','RT04','4','RO01','P408');</v>
-      </c>
-      <c r="C86" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO038','RT04','4','RO01','P408');</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO038','RT04','5','RO01','P508');</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="18.75" customHeight="1">
       <c r="A87" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO039','RT04','5','RO01','P509');</v>
+      </c>
+      <c r="C87" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO039','RT04','4','RO01','P409');</v>
-      </c>
-      <c r="C87" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO039','RT04','4','RO01','P409');</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1">
+        <v>RO039','RT04','5','RO01','P509');</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="18.75" customHeight="1">
       <c r="A88" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO040','RT04','5','RO01','P510');</v>
+      </c>
+      <c r="C88" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO tbl_room( room_id,room_type_id,floor,status_id,room_number) VALUES('RO040','RT04','4','RO01','P410');</v>
-      </c>
-      <c r="C88" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>RO040','RT04','4','RO01','P410');</v>
+        <v>RO040','RT04','5','RO01','P510');</v>
       </c>
     </row>
   </sheetData>
@@ -7089,7 +7091,7 @@
   <dimension ref="A3:O54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A31" sqref="A31:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -7207,10 +7209,10 @@
         <v>129</v>
       </c>
       <c r="E5" s="1">
-        <v>20170825</v>
+        <v>20170831</v>
       </c>
       <c r="F5" s="1">
-        <v>20170829</v>
+        <v>20170902</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -7239,10 +7241,10 @@
         <v>130</v>
       </c>
       <c r="E6" s="1">
-        <v>20170826</v>
+        <v>20170831</v>
       </c>
       <c r="F6" s="1">
-        <v>20170830</v>
+        <v>20170903</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -7271,10 +7273,10 @@
         <v>131</v>
       </c>
       <c r="E7" s="1">
-        <v>20170826</v>
+        <v>20170831</v>
       </c>
       <c r="F7" s="1">
-        <v>20170830</v>
+        <v>20170903</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -7753,31 +7755,31 @@
     <row r="31" spans="1:15">
       <c r="A31" s="23" t="str">
         <f>$C$29&amp;$C$30&amp;C31</f>
-        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,date_in,date_out,customer_name,customer_identity_card,customer_phone,customer_email,note,check_in_flag,check_out_flag,update_ymd,create_ymd) VALUES('1','RO001','20170825','20170829','','','','','','0','0','2017/08/01','2017/08/01');</v>
+        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,date_in,date_out,customer_name,customer_identity_card,customer_phone,customer_email,note,check_in_flag,check_out_flag,update_ymd,create_ymd) VALUES('1','RO001','20170831','20170902','','','','','','0','0','2017/08/01','2017/08/01');</v>
       </c>
       <c r="C31" s="23" t="str">
         <f>""&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"','"&amp;G5&amp;"','"&amp;H5&amp;"','"&amp;I5&amp;"','"&amp;J5&amp;"','"&amp;K5&amp;"','"&amp;L5&amp;"','"&amp;M5&amp;"','"&amp;N5&amp;"','"&amp;O5&amp;"');"</f>
-        <v>1','RO001','20170825','20170829','','','','','','0','0','2017/08/01','2017/08/01');</v>
+        <v>1','RO001','20170831','20170902','','','','','','0','0','2017/08/01','2017/08/01');</v>
       </c>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="23" t="str">
         <f t="shared" ref="A32:A43" si="0">$C$29&amp;$C$30&amp;C32</f>
-        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,date_in,date_out,customer_name,customer_identity_card,customer_phone,customer_email,note,check_in_flag,check_out_flag,update_ymd,create_ymd) VALUES('2','RO002','20170826','20170830','','','','','','0','0','2017/08/02','2017/08/02');</v>
+        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,date_in,date_out,customer_name,customer_identity_card,customer_phone,customer_email,note,check_in_flag,check_out_flag,update_ymd,create_ymd) VALUES('2','RO002','20170831','20170903','','','','','','0','0','2017/08/02','2017/08/02');</v>
       </c>
       <c r="C32" s="23" t="str">
         <f t="shared" ref="C32:C42" si="1">""&amp;C6&amp;"','"&amp;D6&amp;"','"&amp;E6&amp;"','"&amp;F6&amp;"','"&amp;G6&amp;"','"&amp;H6&amp;"','"&amp;I6&amp;"','"&amp;J6&amp;"','"&amp;K6&amp;"','"&amp;L6&amp;"','"&amp;M6&amp;"','"&amp;N6&amp;"','"&amp;O6&amp;"');"</f>
-        <v>2','RO002','20170826','20170830','','','','','','0','0','2017/08/02','2017/08/02');</v>
+        <v>2','RO002','20170831','20170903','','','','','','0','0','2017/08/02','2017/08/02');</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,date_in,date_out,customer_name,customer_identity_card,customer_phone,customer_email,note,check_in_flag,check_out_flag,update_ymd,create_ymd) VALUES('2','RO003','20170826','20170830','','','','','','0','0','2017/08/03','2017/08/03');</v>
+        <v>INSERT INTO tbl_reservation_detail( reservation_id,room_id,date_in,date_out,customer_name,customer_identity_card,customer_phone,customer_email,note,check_in_flag,check_out_flag,update_ymd,create_ymd) VALUES('2','RO003','20170831','20170903','','','','','','0','0','2017/08/03','2017/08/03');</v>
       </c>
       <c r="C33" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>2','RO003','20170826','20170830','','','','','','0','0','2017/08/03','2017/08/03');</v>
+        <v>2','RO003','20170831','20170903','','','','','','0','0','2017/08/03','2017/08/03');</v>
       </c>
     </row>
     <row r="34" spans="1:3">

</xml_diff>